<commit_message>
Connect Island Regions (WIP)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E488797-CD8D-47EE-9A71-19A85695707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E5E94A-1614-4BD0-ACA1-106CCCC7894A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="2304" yWindow="288" windowWidth="18492" windowHeight="11880" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -388,12 +389,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FE500E-F281-4920-BC3F-D4783935BF35}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>12+12</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>200</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>SUM(A1:A3)</f>
+        <v>600</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B1:B3)</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>

<commit_message>
Refactor for recalc with  (WIP)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E5E94A-1614-4BD0-ACA1-106CCCC7894A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C90BAB5-E717-4763-85D4-0DEED0D502B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="288" windowWidth="18492" windowHeight="11880" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="3168" yWindow="84" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -392,13 +393,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49FE500E-F281-4920-BC3F-D4783935BF35}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -410,7 +411,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -418,7 +419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -426,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>SUM(A1:A3)</f>
         <v>600</v>
@@ -445,11 +446,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -457,7 +460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -465,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -473,37 +476,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUMIF(A1:A3,100)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>SUMIF(A1:A3,A2)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUMIF(A1:A3,"2*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8">
-        <f>SEARCH("A","ABC")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <f>SEARCH("B","ABC")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUMIF(B1:B3,"A*",A1:A3)</f>
         <v>300</v>

</xml_diff>

<commit_message>
eval error fix for sheet name
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,16 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C90BAB5-E717-4763-85D4-0DEED0D502B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5AF1B-E14A-43F4-BF14-85E14E211584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3168" yWindow="84" windowWidth="15684" windowHeight="11832" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -397,9 +396,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>100</v>
       </c>
@@ -411,7 +410,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>200</v>
       </c>
@@ -419,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>300</v>
       </c>
@@ -427,7 +426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>SUM(A1:A3)</f>
         <v>600</v>
@@ -447,12 +446,12 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>100</v>
       </c>
@@ -460,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>200</v>
       </c>
@@ -468,7 +467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>300</v>
       </c>
@@ -476,37 +475,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4">
-        <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
+        <f>SUMIF(A1:A3,"&gt;"&amp;A1,A1:A3)</f>
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5">
         <f>SUMIF(A1:A3,100)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6">
         <f>SUMIF(A1:A3,A2)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7">
         <f>SUMIF(A1:A3,"2*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8">
-        <f>SEARCH("B","ABC")</f>
+        <f>SEARCH("B","ABC",1)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9">
         <f>SUMIF(B1:B3,"A*",A1:A3)</f>
         <v>300</v>

</xml_diff>

<commit_message>
wrap <fn>if, countif, averageif, concatenate
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5AF1B-E14A-43F4-BF14-85E14E211584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBE61D-5BFA-4B7D-8DB6-BA29EBFBDA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
@@ -393,7 +393,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -477,7 +477,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4">
-        <f>SUMIF(A1:A3,"&gt;"&amp;A1,A1:A3)</f>
+        <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
         <v>500</v>
       </c>
     </row>
@@ -511,6 +511,30 @@
         <v>300</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <f>AVERAGE(A1:A3)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <f>AVERAGEIF(A1:A3,"&gt;100")</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <f>COUNTIF(A1:A3,"&gt;100")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <f>CONCATENATE(B1,":",B2,":",B3)</f>
+        <v>A:AA:B</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add INDEX (array form)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACBE61D-5BFA-4B7D-8DB6-BA29EBFBDA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B5841E-F63C-4F31-81C8-558D773E94A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="1" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>A</t>
   </si>
@@ -443,10 +444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE7C9D-64A9-4AF9-B04F-DA6586A94AFB}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -535,6 +536,93 @@
         <v>A:AA:B</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <f>INDEX(A1:B3,1,2)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>INDEX(A1:A3,1)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f>INDEX(A1:B1,2)</f>
+        <v>A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E525-1CDF-423A-8DB5-671571BC1298}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>300</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="str">
+        <f>INDEX(A1:B3,1,2)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <f>INDEX(A1:A3,1)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f>INDEX(A1:A3,2)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <f>INDEX(A1:B1,1)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="str">
+        <f>INDEX(A1:B1,2)</f>
+        <v>A</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add infix colon operator, start work on reference macros
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B5841E-F63C-4F31-81C8-558D773E94A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF2B80-A414-4705-8C03-6B326C632BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="3" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -40,13 +41,52 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Apples</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Lemons</t>
+  </si>
+  <si>
+    <t>Oranges</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>Almonds</t>
+  </si>
+  <si>
+    <t>Cashews</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>Walnuts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,16 +94,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="19.2"/>
+      <color rgb="FF393939"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="19.2"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDADADA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F4F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +136,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E525-1CDF-423A-8DB5-671571BC1298}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -626,4 +714,159 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EA1BDB-2DAD-4A3D-9B90-64D5D2FD0A97}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.8984375" customWidth="1"/>
+    <col min="2" max="2" width="41.69921875" customWidth="1"/>
+    <col min="3" max="3" width="21.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="C3" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <f>INDEX(A2:C6, 2, 3)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f>INDEX((A1:C6, A8:C11), 2, 2, 2)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>SUM(INDEX(A1:C11, 0, 3, 1))</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>SUM(B2:INDEX(A2:C6, 5, 2))</f>
+        <v>2.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dynamic construction of ranges (wip)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF2B80-A414-4705-8C03-6B326C632BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F9E6E-6712-49A0-AE20-BA107846FB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="3" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="1920" yWindow="1128" windowWidth="15684" windowHeight="11832" activeTab="3" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Walnuts</t>
+  </si>
+  <si>
+    <t>=INDEX((A1:C6, A8:B10), 2, 3, 2)</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -165,6 +168,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +726,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -846,21 +851,28 @@
         <f>INDEX(A2:C6, 2, 3)</f>
         <v>38</v>
       </c>
+      <c r="B12" s="6">
+        <f>SUM(B4:B6,B6:C6,C6:C8,B9)</f>
+        <v>109.22999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="5">
         <f>INDEX((A1:C6, A8:C11), 2, 2, 2)</f>
         <v>1.25</v>
       </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="5">
         <f>SUM(INDEX(A1:C11, 0, 3, 1))</f>
         <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="5">
         <f>SUM(B2:INDEX(A2:C6, 5, 2))</f>
         <v>2.42</v>
       </c>

</xml_diff>

<commit_message>
dynamic construction of ranges, index, match (wip)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09F9E6E-6712-49A0-AE20-BA107846FB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2699333-5599-4E3A-856E-6EF207F13BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1128" windowWidth="15684" windowHeight="11832" activeTab="3" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="3036" yWindow="180" windowWidth="15684" windowHeight="11832" activeTab="4" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -79,7 +80,7 @@
     <t>Walnuts</t>
   </si>
   <si>
-    <t>=INDEX((A1:C6, A8:B10), 2, 3, 2)</t>
+    <t>Product</t>
   </si>
 </sst>
 </file>
@@ -89,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +107,24 @@
     </font>
     <font>
       <sz val="19.2"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF393939"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF1E1E1E"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -154,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -170,6 +189,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EA1BDB-2DAD-4A3D-9B90-64D5D2FD0A97}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -861,8 +884,9 @@
         <f>INDEX((A1:C6, A8:C11), 2, 2, 2)</f>
         <v>1.25</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>15</v>
+      <c r="B13" s="5">
+        <f>INDEX((A1:C6, A8:B10), 2, 2, 2)</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -875,6 +899,80 @@
       <c r="A15" s="5">
         <f>SUM(B2:INDEX(A2:C6, 5, 2))</f>
         <v>2.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BC19B-F004-474A-8CBD-B3D9192C7A3B}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="7" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="7" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="7" customFormat="1" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <f>MATCH(39,B2:B5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <f>MATCH(41,B2:B5,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="e">
+        <f>MATCH(40,B2:B5,-1)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic construction of ranges, index, match, indirect (wip)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2699333-5599-4E3A-856E-6EF207F13BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B9E45-108A-4019-A1CB-B8BD29CB1A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="180" windowWidth="15684" windowHeight="11832" activeTab="4" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="3840" yWindow="0" windowWidth="15684" windowHeight="11832" activeTab="4" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -14,6 +14,9 @@
     <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="George">Sheet6!$B$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -81,6 +106,15 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
   </si>
 </sst>
 </file>
@@ -909,10 +943,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BC19B-F004-474A-8CBD-B3D9192C7A3B}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -975,6 +1009,68 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" cm="1">
+        <f t="array" aca="1" ref="A16" ca="1">INDIRECT(A11)</f>
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" cm="1">
+        <f t="array" aca="1" ref="A17" ca="1">INDIRECT(A12)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" cm="1">
+        <f t="array" aca="1" ref="A18" ca="1">INDIRECT(A13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" cm="1">
+        <f t="array" aca="1" ref="A19" ca="1">INDIRECT("B"&amp;A14)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" cm="1">
+        <f t="array" aca="1" ref="A20" ca="1">INDIRECT("Sheet6!B"&amp;A14)</f>
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
dynamic construction of ranges etc (boxing)
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792B9E45-108A-4019-A1CB-B8BD29CB1A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5251EAD-41AB-4DF1-B1D4-97CB943F02AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="0" windowWidth="15684" windowHeight="11832" activeTab="4" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="3840" yWindow="0" windowWidth="15684" windowHeight="11832" activeTab="5" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="George">Sheet6!$B$13</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>A</t>
   </si>
@@ -115,6 +116,27 @@
   </si>
   <si>
     <t>B12</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Displays the value in cell B6 (4)</t>
+  </si>
+  <si>
+    <t>Sums the range B6:D8</t>
+  </si>
+  <si>
+    <t>Returns an error, because the reference is to a non-existent range on the worksheet.</t>
   </si>
 </sst>
 </file>
@@ -945,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BC19B-F004-474A-8CBD-B3D9192C7A3B}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -1075,4 +1097,100 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6577517-334F-42B2-B8A8-54768A941DD3}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f ca="1">OFFSET(D3,3,-2,1,1)</f>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f ca="1">SUM(OFFSET(D3:F5,3,-2, 3, 3))</f>
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="e">
+        <f ca="1">OFFSET(D3, -3, -3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Many improvements to indirect access, named ranges and function coverage (#3)
* add infix colon operator, start work on reference macros

* dynamic construction of ranges (wip)

* dynamic construction of ranges, index, match (wip)

* dynamic construction of ranges, index, match, indirect (wip)

* dynamic construction of ranges etc (boxing)

* dynamic construction of ranges etc (boxing)

* dynamic construction of ranges etc (dates, pmt)

* hidden names

* scoped named refs
</commit_message>
<xml_diff>
--- a/resources/TEST-cyclic.xlsx
+++ b/resources/TEST-cyclic.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B5841E-F63C-4F31-81C8-558D773E94A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6329A92-7021-419F-A7E0-FDBD59CD7AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="18648" windowHeight="11112" activeTab="2" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{192190A1-2DD6-EF40-BB78-B88DBE69CAA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet7" sheetId="8" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="George" localSheetId="4">Sheet6!$B$13</definedName>
+    <definedName name="George">Sheet6!$B$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>A</t>
   </si>
@@ -40,13 +69,88 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Apples</t>
+  </si>
+  <si>
+    <t>Bananas</t>
+  </si>
+  <si>
+    <t>Lemons</t>
+  </si>
+  <si>
+    <t>Oranges</t>
+  </si>
+  <si>
+    <t>Pears</t>
+  </si>
+  <si>
+    <t>Almonds</t>
+  </si>
+  <si>
+    <t>Cashews</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>Walnuts</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Displays the value in cell B6 (4)</t>
+  </si>
+  <si>
+    <t>Sums the range B6:D8</t>
+  </si>
+  <si>
+    <t>Returns an error, because the reference is to a non-existent range on the worksheet.</t>
+  </si>
+  <si>
+    <t>Local George</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,16 +158,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="19.2"/>
+      <color rgb="FF393939"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="19.2"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF393939"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDADADA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F4F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +218,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,9 +573,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -411,7 +587,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -419,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -427,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>SUM(A1:A3)</f>
         <v>600</v>
@@ -450,9 +626,9 @@
       <selection activeCell="B16" sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -460,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -468,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -476,79 +652,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>SUMIF(A1:A3,"&gt;"&amp;A1)</f>
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUMIF(A1:A3,100)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>SUMIF(A1:A3,A2)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUMIF(A1:A3,"2*")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>SEARCH("B","ABC",1)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>SUMIF(B1:B3,"A*",A1:A3)</f>
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>AVERAGE(A1:A3)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>AVERAGEIF(A1:A3,"&gt;100")</f>
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>COUNTIF(A1:A3,"&gt;100")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>CONCATENATE(B1,":",B2,":",B3)</f>
         <v>A:AA:B</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>INDEX(A1:B3,1,2)</f>
         <v>A</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>INDEX(A1:A3,1)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>INDEX(A1:B1,2)</f>
         <v>A</v>
@@ -563,13 +739,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3100E525-1CDF-423A-8DB5-671571BC1298}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -577,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>200</v>
       </c>
@@ -585,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>300</v>
       </c>
@@ -593,31 +769,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>INDEX(A1:B3,1,2)</f>
         <v>A</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>INDEX(A1:A3,1)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>INDEX(A1:A3,2)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>INDEX(A1:B1,1)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f>INDEX(A1:B1,2)</f>
         <v>A</v>
@@ -626,4 +802,410 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33EA1BDB-2DAD-4A3D-9B90-64D5D2FD0A97}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.875" customWidth="1"/>
+    <col min="2" max="2" width="41.75" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="C2" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="C3" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="C5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3.55</v>
+      </c>
+      <c r="C8" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C9" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="C10" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <f>INDEX(A2:C6, 2, 3)</f>
+        <v>38</v>
+      </c>
+      <c r="B12" s="6">
+        <f>SUM(B4:B6,B6:C6,C6:C8,B9)</f>
+        <v>109.22999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f>INDEX((A1:C6, A8:C11), 2, 2, 2)</f>
+        <v>1.25</v>
+      </c>
+      <c r="B13" s="5">
+        <f>INDEX((A1:C6, A8:B10), 2, 2, 2)</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f>SUM(INDEX(A1:C11, 0, 3, 1))</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f>SUM(B2:INDEX(A2:C6, 5, 2))</f>
+        <v>2.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303BC19B-F004-474A-8CBD-B3D9192C7A3B}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="7" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="7" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="7" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="7" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <f>MATCH(39,B2:B5,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <f>MATCH(41,B2:B5,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="e">
+        <f>MATCH(40,B2:B5,-1)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" cm="1">
+        <f t="array" aca="1" ref="A17" ca="1">INDIRECT(A11)</f>
+        <v>1.333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" cm="1">
+        <f t="array" aca="1" ref="A18" ca="1">INDIRECT(A12)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" cm="1">
+        <f t="array" aca="1" ref="A19" ca="1">INDIRECT(A14)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" cm="1">
+        <f t="array" aca="1" ref="A20" ca="1">INDIRECT("B"&amp;A15)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" cm="1">
+        <f t="array" aca="1" ref="A21" ca="1">INDIRECT("Sheet6!B"&amp;A15)</f>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6577517-334F-42B2-B8A8-54768A941DD3}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="73.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f ca="1">OFFSET(D3,3,-2,1,1)</f>
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f ca="1">SUM(OFFSET(D3:F5,3,-2, 3, 3))</f>
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="e">
+        <f ca="1">OFFSET(D3, -3, -3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>